<commit_message>
Remove extraneous ETL CSV test resources. Update ETL CSV test resources to remove unsupported characters.
</commit_message>
<xml_diff>
--- a/org.matonto.etl.csv/src/test/resources/testFile.xlsx
+++ b/org.matonto.etl.csv/src/test/resources/testFile.xlsx
@@ -20,93 +20,90 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>Material</t>
-  </si>
-  <si>
-    <t>Crystal structure</t>
-  </si>
-  <si>
-    <t>Lattice parameters a(�)</t>
-  </si>
-  <si>
-    <t>b(�)</t>
-  </si>
-  <si>
-    <t>c(�)</t>
-  </si>
-  <si>
-    <t>Density(g/mL)</t>
-  </si>
-  <si>
-    <t>Melting point (�C)</t>
-  </si>
-  <si>
-    <t>Melting point (�F)</t>
-  </si>
-  <si>
-    <t>http://en.wikipedia.org/wiki/Ultra-high-temperature_ceramics</t>
-  </si>
-  <si>
-    <t>HfB2</t>
-  </si>
-  <si>
-    <t>Hexagonal</t>
-  </si>
-  <si>
-    <t>�</t>
-  </si>
-  <si>
-    <t>HfC</t>
-  </si>
-  <si>
-    <t>FCC</t>
-  </si>
-  <si>
-    <t>HfN</t>
-  </si>
-  <si>
-    <t>ZrB2</t>
-  </si>
-  <si>
-    <t>ZrC</t>
-  </si>
-  <si>
-    <t>ZrN</t>
-  </si>
-  <si>
-    <t>TiB2</t>
-  </si>
-  <si>
-    <t>TiC</t>
-  </si>
-  <si>
-    <t>Cubic</t>
-  </si>
-  <si>
-    <t>TiN</t>
-  </si>
-  <si>
-    <t>TaB2</t>
-  </si>
-  <si>
-    <t>TaC</t>
-  </si>
-  <si>
-    <t>TaN</t>
-  </si>
-  <si>
-    <t>SiC</t>
-  </si>
-  <si>
-    <t>Polymorphic</t>
-  </si>
-  <si>
-    <t>Various</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
+  <si>
+    <t xml:space="preserve">Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crystal structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lattice parameters a(Å)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b(Å)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c(Å)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Density(g/mL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melting point (°C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melting point (°F)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://en.wikipedia.org/wiki/Ultra-high-temperature_ceramics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HfB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hexagonal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HfC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HfN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZrB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZrC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZrN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TiB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TiC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cubic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TiN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TaB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TaC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TaN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SiC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polymorphic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Various</t>
   </si>
 </sst>
 </file>
@@ -114,13 +111,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -180,8 +178,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -205,24 +207,24 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.79591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.6938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.7551020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.30612244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.85714285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.7602040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.2704081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.0255102040816"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.67857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.7602040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.19897959183674"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.87755102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.7142857142857"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.3265306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.0714285714286"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -232,26 +234,26 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>9</v>
       </c>
@@ -261,16 +263,16 @@
       <c r="C2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>3.142</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="0" t="n">
+      <c r="E2" s="1" t="n">
+        <v>3.321</v>
+      </c>
+      <c r="F2" s="1" t="n">
         <v>3.476</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>11.19</v>
       </c>
       <c r="H2" s="0" t="n">
@@ -280,26 +282,26 @@
         <v>6116</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>4.638</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>4.638</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>4.638</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>12.76</v>
       </c>
       <c r="H3" s="0" t="n">
@@ -309,26 +311,26 @@
         <v>7052</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="n">
         <v>4.525</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>4.525</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>4.525</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>13.9</v>
       </c>
       <c r="H4" s="0" t="n">
@@ -338,26 +340,26 @@
         <v>6125</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>3.169</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="0" t="n">
+      <c r="E5" s="1" t="n">
+        <v>3.333</v>
+      </c>
+      <c r="F5" s="1" t="n">
         <v>3.53</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <v>6.1</v>
       </c>
       <c r="H5" s="0" t="n">
@@ -367,26 +369,26 @@
         <v>5873</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="n">
         <v>4.693</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>4.693</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>4.693</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <v>6.56</v>
       </c>
       <c r="H6" s="0" t="n">
@@ -396,26 +398,26 @@
         <v>6152</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="n">
         <v>4.578</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>4.578</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>4.578</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>7.29</v>
       </c>
       <c r="H7" s="0" t="n">
@@ -425,26 +427,26 @@
         <v>5342</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>3.03</v>
       </c>
-      <c r="E8" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="0" t="n">
+      <c r="E8" s="1" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="F8" s="1" t="n">
         <v>3.23</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <v>4.52</v>
       </c>
       <c r="H8" s="0" t="n">
@@ -454,26 +456,26 @@
         <v>5837</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>4.327</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>4.327</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <v>4.327</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>4.94</v>
       </c>
       <c r="H9" s="0" t="n">
@@ -483,26 +485,26 @@
         <v>5612</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1" t="n">
         <v>4.242</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>4.242</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <v>4.242</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>5.39</v>
       </c>
       <c r="H10" s="0" t="n">
@@ -512,26 +514,26 @@
         <v>5342</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>3.098</v>
       </c>
-      <c r="E11" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="0" t="n">
+      <c r="E11" s="1" t="n">
+        <v>3.142</v>
+      </c>
+      <c r="F11" s="1" t="n">
         <v>3.227</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="1" t="n">
         <v>12.54</v>
       </c>
       <c r="H11" s="0" t="n">
@@ -541,26 +543,26 @@
         <v>5504</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1" t="n">
         <v>4.455</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>4.455</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="1" t="n">
         <v>4.455</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="1" t="n">
         <v>14.5</v>
       </c>
       <c r="H12" s="0" t="n">
@@ -570,26 +572,26 @@
         <v>6872</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D13" s="1" t="n">
         <v>4.33</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>4.33</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="1" t="n">
         <v>4.33</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="1" t="n">
         <v>14.3</v>
       </c>
       <c r="H13" s="0" t="n">
@@ -599,26 +601,26 @@
         <v>4892</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="D14" s="1" t="n">
+        <v>4.65</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="0" t="n">
+      <c r="F14" s="1" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="G14" s="1" t="n">
         <v>3.21</v>
       </c>
       <c r="H14" s="0" t="n">

</xml_diff>